<commit_message>
terminando configuracion del contenedor
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kerberos/Desktop/testv5/azure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D845795-147A-964A-A22E-3BA2D1BA54E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE034D7-036E-0C49-B2FC-66E172C9B35E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>id_managemeet</t>
   </si>
@@ -83,13 +83,28 @@
   </si>
   <si>
     <t>https://comfama.webex.com/comfama/ldr.php?RCID=24172b94001615a9f9924cc1be32e5eddd</t>
+  </si>
+  <si>
+    <t>Idiomas: B2:Inglés intermedio, N15 (J-Ad13+)</t>
+  </si>
+  <si>
+    <t>Yoeimis Paola Polo Gutiérrez</t>
+  </si>
+  <si>
+    <t>YoeimisPolo@comfama.com.co</t>
+  </si>
+  <si>
+    <t>Clase 20 - 53068055</t>
+  </si>
+  <si>
+    <t>https://comfama.webex.com/comfama/ldr.php?RCID=89c0e2e34c9e0ecbbbb3051d1027ddfc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,6 +243,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0066CC"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -575,11 +598,12 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -936,10 +960,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1087,6 +1111,41 @@
         <v>15</v>
       </c>
     </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>84470</v>
+      </c>
+      <c r="B5">
+        <v>53068055</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="1">
+        <v>44527</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="I5">
+        <v>8360</v>
+      </c>
+      <c r="J5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K3" r:id="rId1" xr:uid="{0F2A87DD-B3A3-AF42-813D-1511523E3117}"/>

</xml_diff>

<commit_message>
creando archivos de aprovisionamiento de ansible
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kerberos/Desktop/testv5/azure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE034D7-036E-0C49-B2FC-66E172C9B35E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0B4BC2-F837-1B44-9C09-9D31E2F4BF96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1100" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="enviado_para_prueba" sheetId="1" r:id="rId1"/>
@@ -963,7 +963,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A3" sqref="A3:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>